<commit_message>
Se cambiaron los documentos de estados financieros del primer trimestre 2023
</commit_message>
<xml_diff>
--- a/src/assets/content/estados-financieros/2023/primer-trimestre/02_INFORMACION_PRESUPUESTARIA/03_ESTADO_ANALITICO_DE_EGRESOS_CLASIFICACION_ECONOMICA.xlsx
+++ b/src/assets/content/estados-financieros/2023/primer-trimestre/02_INFORMACION_PRESUPUESTARIA/03_ESTADO_ANALITICO_DE_EGRESOS_CLASIFICACION_ECONOMICA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1.- EJERCICIO 2023\1.1ER TRIMESTRE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1.- EJERCICIO 2023\1.1ER TRIMESTRE\SAP HANA\INFORMACION FINANCIERA V2\2.-INFORMACION PRESUPUESTARIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDFFE9C8-4E5D-4144-91A1-90DCF981E496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B28B1F71-555B-4CD8-995C-EBBE8C731475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{69993DDB-D403-4589-BBDE-B97E8772EE24}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{43091E5C-B075-458B-9C6E-85680B679BC2}"/>
   </bookViews>
   <sheets>
     <sheet name="CTG" sheetId="1" r:id="rId1"/>
@@ -36,23 +36,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>UNIVERSIDAD TECNOLOGICA DE SALAMANCA
 Estado Analítico del Ejercicio del Presupuesto de Egresos
-Clasificación Económica (por Tipo de Gasto)
+Clasificación Economica (por Tipo del Gasto) 
 Del 1 de Enero al 31 de Marzo de 2023</t>
   </si>
   <si>
+    <t>Egresos</t>
+  </si>
+  <si>
+    <t>Subejercicio</t>
+  </si>
+  <si>
     <t>Concepto</t>
   </si>
   <si>
-    <t>Egresos</t>
-  </si>
-  <si>
-    <t>Subejercicio</t>
-  </si>
-  <si>
     <t>Aprobado</t>
   </si>
   <si>
@@ -90,40 +90,18 @@
   </si>
   <si>
     <t>Total del Gasto</t>
-  </si>
-  <si>
-    <t>“Bajo protesta de decir verdad declaramos que los Estados Financieros y sus notas, son razonablemente correctos y son responsabilidad del emisor”</t>
-  </si>
-  <si>
-    <t>Josué Calzada Razo</t>
-  </si>
-  <si>
-    <t>Fernando Trujillo Jiménez</t>
-  </si>
-  <si>
-    <t>Encargado de la Direccion de Administracion y Finanzas</t>
-  </si>
-  <si>
-    <t>Rector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,45 +117,11 @@
     </font>
     <font>
       <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,8 +134,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -200,6 +150,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -213,8 +198,25 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -224,104 +226,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -360,109 +270,84 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="4" xr:uid="{95E1BA97-9589-45F0-A941-1A419380A93E}"/>
-    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{833376A2-99F5-4AD4-8341-DEB0BE6670C6}"/>
-    <cellStyle name="Normal 2 3" xfId="3" xr:uid="{3FD5338A-48E7-4076-A11F-2C7BE512757F}"/>
-    <cellStyle name="Normal 3 2" xfId="1" xr:uid="{4C364D2A-31AE-4EA5-8BDB-88237F5D949E}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{C57A14CB-C5C2-4066-A3DA-8AFBDB98E4C6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,291 +658,306 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9202EF5-E741-434E-AA3D-8AA69F3673D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95ED63D5-D336-4675-AD4D-F19BBFDA70D2}">
   <sheetPr>
-    <tabColor rgb="FF00B050"/>
+    <tabColor theme="7" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:I19"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" style="4"/>
-    <col min="2" max="2" width="3" style="4" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" style="4" customWidth="1"/>
-    <col min="4" max="9" width="18.28515625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="12" style="4"/>
+    <col min="1" max="1" width="47.7109375" style="3" customWidth="1"/>
+    <col min="2" max="7" width="18.28515625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="12" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="1" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="7" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14">
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="E5" s="14">
+      <c r="C4" s="14">
         <v>2</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="14">
+      <c r="E4" s="14">
         <v>4</v>
       </c>
-      <c r="H5" s="14">
+      <c r="F4" s="14">
         <v>5</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="15"/>
-      <c r="C6" s="16" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="17">
+      <c r="B6" s="18">
         <v>54130973.5</v>
       </c>
-      <c r="E6" s="17">
+      <c r="C6" s="18">
         <v>1808760.5</v>
       </c>
-      <c r="F6" s="17">
+      <c r="D6" s="18">
+        <f>B6+C6</f>
         <v>55939734</v>
       </c>
-      <c r="G6" s="17">
+      <c r="E6" s="18">
         <v>11120242.65</v>
       </c>
-      <c r="H6" s="17">
-        <v>11120238.41</v>
-      </c>
-      <c r="I6" s="17">
+      <c r="F6" s="18">
+        <v>11120242.65</v>
+      </c>
+      <c r="G6" s="18">
+        <f>D6-E6</f>
         <v>44819491.350000001</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="15"/>
-      <c r="C7" s="16" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="17">
-        <v>0</v>
-      </c>
-      <c r="E7" s="17">
+      <c r="B8" s="18">
+        <v>0</v>
+      </c>
+      <c r="C8" s="18">
         <v>4199216.99</v>
       </c>
-      <c r="F7" s="17">
+      <c r="D8" s="18">
+        <f>B8+C8</f>
         <v>4199216.99</v>
       </c>
-      <c r="G7" s="17">
-        <v>0</v>
-      </c>
-      <c r="H7" s="17">
-        <v>0</v>
-      </c>
-      <c r="I7" s="17">
+      <c r="E8" s="18">
+        <v>0</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0</v>
+      </c>
+      <c r="G8" s="18">
+        <f>D8-E8</f>
         <v>4199216.99</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="15"/>
-      <c r="C8" s="16" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="17">
-        <v>0</v>
-      </c>
-      <c r="E8" s="17">
-        <v>0</v>
-      </c>
-      <c r="F8" s="17">
-        <v>0</v>
-      </c>
-      <c r="G8" s="17">
-        <v>0</v>
-      </c>
-      <c r="H8" s="17">
-        <v>0</v>
-      </c>
-      <c r="I8" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="15"/>
-      <c r="C9" s="16" t="s">
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18">
+        <v>0</v>
+      </c>
+      <c r="D10" s="18">
+        <f>B10+C10</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0</v>
+      </c>
+      <c r="G10" s="18">
+        <f>D10-E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="17">
-        <v>0</v>
-      </c>
-      <c r="E9" s="17">
-        <v>0</v>
-      </c>
-      <c r="F9" s="17">
-        <v>0</v>
-      </c>
-      <c r="G9" s="17">
-        <v>0</v>
-      </c>
-      <c r="H9" s="17">
-        <v>0</v>
-      </c>
-      <c r="I9" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="15"/>
-      <c r="C10" s="18" t="s">
+      <c r="B12" s="18">
+        <v>0</v>
+      </c>
+      <c r="C12" s="18">
+        <v>0</v>
+      </c>
+      <c r="D12" s="18">
+        <f>B12+C12</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0</v>
+      </c>
+      <c r="F12" s="18">
+        <v>0</v>
+      </c>
+      <c r="G12" s="18">
+        <f>D12-E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="19">
-        <v>0</v>
-      </c>
-      <c r="E10" s="19">
-        <v>0</v>
-      </c>
-      <c r="F10" s="19">
-        <v>0</v>
-      </c>
-      <c r="G10" s="19">
-        <v>0</v>
-      </c>
-      <c r="H10" s="19">
-        <v>0</v>
-      </c>
-      <c r="I10" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="21" t="s">
+      <c r="B14" s="18">
+        <v>0</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0</v>
+      </c>
+      <c r="D14" s="18">
+        <f>B14+C14</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0</v>
+      </c>
+      <c r="F14" s="18">
+        <v>0</v>
+      </c>
+      <c r="G14" s="18">
+        <f>D14-E14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="22">
+      <c r="B16" s="22">
+        <f t="shared" ref="B16:G16" si="0">SUM(B6+B8+B10+B12+B14)</f>
         <v>54130973.5</v>
       </c>
-      <c r="E11" s="22">
+      <c r="C16" s="22">
+        <f t="shared" si="0"/>
         <v>6007977.4900000002</v>
       </c>
-      <c r="F11" s="22">
+      <c r="D16" s="22">
+        <f t="shared" si="0"/>
         <v>60138950.990000002</v>
       </c>
-      <c r="G11" s="22">
+      <c r="E16" s="22">
+        <f t="shared" si="0"/>
         <v>11120242.65</v>
       </c>
-      <c r="H11" s="22">
-        <v>11120238.41</v>
-      </c>
-      <c r="I11" s="22">
+      <c r="F16" s="22">
+        <f t="shared" si="0"/>
+        <v>11120242.65</v>
+      </c>
+      <c r="G16" s="22">
+        <f t="shared" si="0"/>
         <v>49018708.340000004</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="12" x14ac:dyDescent="0.2">
-      <c r="C17" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="3:8" ht="11.4" x14ac:dyDescent="0.2">
-      <c r="C18" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="27"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" autoFilter="0"/>
-  <mergeCells count="8">
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:C5"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="141" scale="96" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="141" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>